<commit_message>
Multi style and config
</commit_message>
<xml_diff>
--- a/datatest.xlsx
+++ b/datatest.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TanInterIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C853C3A7-CE50-4FCF-8B39-45212E552CC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C666E9-DAEB-4D6B-8B98-C9A5E9F7BB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Style1" sheetId="1" r:id="rId1"/>
+    <sheet name="Style2" sheetId="3" r:id="rId2"/>
     <sheet name="OPERATION_CONFIG" sheetId="2" r:id="rId3"/>
     <sheet name="NO_WIP_REQ" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>sequence</t>
   </si>
@@ -74,28 +74,25 @@
     <t>WIP</t>
   </si>
   <si>
-    <t>OPERATION</t>
-  </si>
-  <si>
-    <t>NEXT_OPERATION</t>
-  </si>
-  <si>
     <t>Sew Center</t>
   </si>
   <si>
     <t>Topstitch</t>
   </si>
   <si>
-    <t>STYLE 1</t>
-  </si>
-  <si>
-    <t>STYLE</t>
-  </si>
-  <si>
-    <t>STYLE 2</t>
-  </si>
-  <si>
     <t>Attach Sling Rubber</t>
+  </si>
+  <si>
+    <t>style</t>
+  </si>
+  <si>
+    <t>Style 1</t>
+  </si>
+  <si>
+    <t>Style 2</t>
+  </si>
+  <si>
+    <t>next operation</t>
   </si>
 </sst>
 </file>
@@ -553,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7D4BD3B-9398-4D8C-A255-CA64E6C0981D}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B10"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -619,7 +616,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>6</v>
@@ -636,7 +633,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>8</v>
@@ -653,7 +650,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C6">
         <v>4</v>
@@ -743,7 +740,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -755,13 +752,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -777,46 +774,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -828,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81ADBA82-A88C-4428-9B3D-C47BDAA8E87C}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -839,10 +836,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -863,7 +860,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -871,7 +868,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -879,10 +876,10 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>